<commit_message>
update result & plan
</commit_message>
<xml_diff>
--- a/2021년/20210104.xlsx
+++ b/2021년/20210104.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\2021년\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2360EB66-1F0D-4F5A-A1A8-26A48FD2FBB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625CABFD-B5F7-4E61-BE91-8C4B9699D9C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>일</t>
   </si>
@@ -166,10 +166,6 @@
   </si>
   <si>
     <t>주간 목표</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">금일 업무 </t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
@@ -210,21 +206,129 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>1. stm32 relay wifi
- - 사양관련 회의
-  -&gt; 추가사항 반영</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>relay관련 회의, dev kit 품목선정</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>relay_wifi 추가회로 마무리</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>추가 풋프린트 마무리</t>
+    <t>회로 마무리</t>
+  </si>
+  <si>
+    <t>회로 마무리</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>아트웍</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 일정</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>회로 &amp; 풋프린트 마무리</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>부품 선정 &amp; 발주</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>릴레이 보드 회로설계</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨트롤러 보드 테스트</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>릴레이보드 아트웍</t>
+  </si>
+  <si>
+    <t>릴레이보드 아트웍</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>릴레이보드 아트웍 &amp; PCB발주</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>릴레이 보드 부품선정 &amp; 부품발주</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>릴레이보드 테스트 프로그램 제작</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨트롤러 보드 테스트프로그램 제작</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨트롤러 wifi테스트 &amp; 아트웍</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨트롤러 아트웍</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>컨트롤러 아트웍 &amp; PCB발주</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>buffer</t>
+  </si>
+  <si>
+    <t>buffer</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>보드 테스트</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. SCR-OBD
+ - 부저 추가
+  -&gt; 기존버젼과 60set납품버젼의 회로도가 달라 cubemx수정
+   =&gt; 기존 LED output으로 사용하였던 핀중 Timer2 CH2에 PWM핀이 하나 남아서 사용함
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>==&gt; 소리가 너무작아서 MLT에 Active Buzzer로 쪽보드 제작 의뢰</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+2. STM32_RELAY_WIFI
+ - 아웃풋 4EA추가 설계 완료
+  -&gt; ULN2803사용하여 오픈콜렉터 형식으로 4채널 출력
+ - 디버깅 (진행중)
+  -&gt; 회로에서 PCB로 넘기기 위해 각종 핀에러 수정 및 Footpring매칭 
+3. 2020년 프로젝트 결산
+ - 프로젝트 참여비율 계산 및 결과 전달 (To GD)</t>
+    </r>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -235,7 +339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -404,8 +508,16 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -610,8 +722,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -778,6 +932,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -913,7 +1093,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -923,30 +1103,6 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -956,21 +1112,6 @@
     <xf numFmtId="0" fontId="22" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="1" fillId="32" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -988,6 +1129,75 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="23" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="23" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="41" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1519,9 +1729,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:M23"/>
+  <dimension ref="B2:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E23"/>
     </sheetView>
   </sheetViews>
@@ -1531,15 +1741,17 @@
     <col min="3" max="3" width="63.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.125" customWidth="1"/>
     <col min="5" max="5" width="85.75" customWidth="1"/>
-    <col min="6" max="6" width="25.125" customWidth="1"/>
-    <col min="7" max="7" width="16.25" customWidth="1"/>
-    <col min="8" max="8" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.75" customWidth="1"/>
-    <col min="11" max="11" width="9.875" customWidth="1"/>
-    <col min="12" max="12" width="78" customWidth="1"/>
+    <col min="6" max="6" width="12.75" customWidth="1"/>
+    <col min="7" max="7" width="85.75" customWidth="1"/>
+    <col min="8" max="8" width="25.125" customWidth="1"/>
+    <col min="9" max="9" width="16.25" customWidth="1"/>
+    <col min="10" max="10" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.75" customWidth="1"/>
+    <col min="13" max="13" width="9.875" customWidth="1"/>
+    <col min="14" max="14" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1550,344 +1762,475 @@
         <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="20">
+        <v>44200</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="15">
+        <v>44201</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="15">
+        <v>44202</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="15">
+        <v>44203</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <f>SUM(L3:L6)</f>
+        <v>206</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="15">
+        <v>44204</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="16">
+        <v>44207</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="16">
+        <v>44208</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="16">
+        <v>44209</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="16">
+        <v>44210</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="16">
+        <v>44211</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="17">
+        <v>44214</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="17">
+        <v>44215</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="17">
+        <v>44216</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="17">
+        <v>44217</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="2:10" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="17">
+        <v>44218</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>7</v>
-      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="18">
+        <v>44221</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
     </row>
-    <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="18">
+        <v>44222</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="34"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="18">
+        <v>44223</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="34"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="18">
+        <v>44224</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="C23" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="15"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="15"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="15"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7">
-        <f>SUM(J3:J6)</f>
-        <v>206</v>
-      </c>
-      <c r="L7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="15"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-    </row>
-    <row r="15" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="18">
+        <v>44225</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="H3:H23"/>
+  <mergeCells count="8">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J3:J23"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="D3:D8"/>
     <mergeCell ref="E3:E23"/>
-    <mergeCell ref="G3:G23"/>
-    <mergeCell ref="F3:F23"/>
+    <mergeCell ref="I3:I23"/>
+    <mergeCell ref="H3:H23"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>